<commit_message>
updated data file (still 1/5, added city variable)
</commit_message>
<xml_diff>
--- a/SLO_Real_Estate_Feb-Apr2022.xlsx
+++ b/SLO_Real_Estate_Feb-Apr2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelroggenkemper/Documents/STAT334/Project/regress_and_depress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BEEAD0-4CCF-1C40-8A54-CBD0E4610F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E270D7-4C4A-B64E-B2B7-66412BCE172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{55ACE583-2BB0-784E-ACAF-9BB688D7FEAA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{55ACE583-2BB0-784E-ACAF-9BB688D7FEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="14">
   <si>
     <t>Sqft</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Cooling</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>San Luis Obispo</t>
   </si>
 </sst>
 </file>
@@ -425,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F185D2F3-BFB7-0647-BBFF-BC17FD9DDBFC}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="94" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -464,8 +470,11 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1435000</v>
       </c>
@@ -496,8 +505,11 @@
       <c r="J2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>711000</v>
       </c>
@@ -528,8 +540,11 @@
       <c r="J3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1603000</v>
       </c>
@@ -560,8 +575,11 @@
       <c r="J4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2100000</v>
       </c>
@@ -592,8 +610,11 @@
       <c r="J5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1394000</v>
       </c>
@@ -624,8 +645,11 @@
       <c r="J6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1035000</v>
       </c>
@@ -656,8 +680,11 @@
       <c r="J7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1500000</v>
       </c>
@@ -688,8 +715,11 @@
       <c r="J8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>255000</v>
       </c>
@@ -720,8 +750,11 @@
       <c r="J9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>760000</v>
       </c>
@@ -752,8 +785,11 @@
       <c r="J10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>820000</v>
       </c>
@@ -784,8 +820,11 @@
       <c r="J11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2323000</v>
       </c>
@@ -816,8 +855,11 @@
       <c r="J12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>990000</v>
       </c>
@@ -848,8 +890,11 @@
       <c r="J13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>936000</v>
       </c>
@@ -880,8 +925,11 @@
       <c r="J14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1000000</v>
       </c>
@@ -912,8 +960,11 @@
       <c r="J15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>668000</v>
       </c>
@@ -944,8 +995,11 @@
       <c r="J16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1200000</v>
       </c>
@@ -976,8 +1030,11 @@
       <c r="J17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>255500</v>
       </c>
@@ -1008,8 +1065,11 @@
       <c r="J18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2405000</v>
       </c>
@@ -1040,8 +1100,11 @@
       <c r="J19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1300000</v>
       </c>
@@ -1072,8 +1135,11 @@
       <c r="J20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>860000</v>
       </c>
@@ -1104,8 +1170,11 @@
       <c r="J21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>838000</v>
       </c>
@@ -1136,8 +1205,11 @@
       <c r="J22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>307000</v>
       </c>
@@ -1168,8 +1240,11 @@
       <c r="J23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1570500</v>
       </c>
@@ -1200,8 +1275,11 @@
       <c r="J24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1514850</v>
       </c>
@@ -1232,8 +1310,11 @@
       <c r="J25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>515000</v>
       </c>
@@ -1264,8 +1345,11 @@
       <c r="J26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1248000</v>
       </c>
@@ -1296,8 +1380,11 @@
       <c r="J27" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>300000</v>
       </c>
@@ -1328,8 +1415,11 @@
       <c r="J28" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>650000</v>
       </c>
@@ -1360,8 +1450,11 @@
       <c r="J29" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1250000</v>
       </c>
@@ -1392,8 +1485,11 @@
       <c r="J30" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1110000</v>
       </c>
@@ -1424,8 +1520,11 @@
       <c r="J31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>950000</v>
       </c>
@@ -1456,8 +1555,11 @@
       <c r="J32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>734000</v>
       </c>
@@ -1488,8 +1590,11 @@
       <c r="J33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>415000</v>
       </c>
@@ -1520,8 +1625,11 @@
       <c r="J34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>876000</v>
       </c>
@@ -1552,8 +1660,11 @@
       <c r="J35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1435000</v>
       </c>
@@ -1584,8 +1695,11 @@
       <c r="J36" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>69000</v>
       </c>
@@ -1616,8 +1730,11 @@
       <c r="J37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1531000</v>
       </c>
@@ -1648,8 +1765,11 @@
       <c r="J38" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1080000</v>
       </c>
@@ -1679,6 +1799,9 @@
       </c>
       <c r="J39" t="s">
         <v>8</v>
+      </c>
+      <c r="K39" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final updated data set with houses sold in SLO from February 2022 - April 2022
</commit_message>
<xml_diff>
--- a/SLO_Real_Estate_Feb-Apr2022.xlsx
+++ b/SLO_Real_Estate_Feb-Apr2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelroggenkemper/Documents/STAT334/Project/regress_and_depress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E270D7-4C4A-B64E-B2B7-66412BCE172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494CF049-53F3-5449-8EF1-E25D307ECBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{55ACE583-2BB0-784E-ACAF-9BB688D7FEAA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="22">
   <si>
     <t>Sqft</t>
   </si>
@@ -73,10 +73,34 @@
     <t>Cooling</t>
   </si>
   <si>
-    <t>City</t>
+    <t>HomeType</t>
   </si>
   <si>
-    <t>San Luis Obispo</t>
+    <t>Condominium</t>
+  </si>
+  <si>
+    <t>SingleFamilyResidence</t>
+  </si>
+  <si>
+    <t>MobileManufactured</t>
+  </si>
+  <si>
+    <t>ManufacturedHome</t>
+  </si>
+  <si>
+    <t>Triplex</t>
+  </si>
+  <si>
+    <t>Duplex</t>
+  </si>
+  <si>
+    <t>PlannedDevelopment</t>
+  </si>
+  <si>
+    <t>MultiFamily</t>
+  </si>
+  <si>
+    <t>Townhouse</t>
   </si>
 </sst>
 </file>
@@ -431,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F185D2F3-BFB7-0647-BBFF-BC17FD9DDBFC}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="94" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -529,7 +553,7 @@
         <v>9645</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -541,7 +565,7 @@
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -576,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -611,7 +635,7 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -646,7 +670,7 @@
         <v>8</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -669,7 +693,7 @@
         <v>8974</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
@@ -681,7 +705,7 @@
         <v>8</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -716,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -739,7 +763,7 @@
         <v>2500</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
@@ -751,7 +775,7 @@
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -786,7 +810,7 @@
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -856,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -891,7 +915,7 @@
         <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -926,7 +950,7 @@
         <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -961,7 +985,7 @@
         <v>8</v>
       </c>
       <c r="K15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1031,7 +1055,7 @@
         <v>8</v>
       </c>
       <c r="K17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1054,7 +1078,7 @@
         <v>1095</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="s">
         <v>8</v>
@@ -1066,7 +1090,7 @@
         <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1101,7 +1125,7 @@
         <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1136,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1171,7 +1195,7 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1206,7 +1230,7 @@
         <v>8</v>
       </c>
       <c r="K22" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1229,7 +1253,7 @@
         <v>1565</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="s">
         <v>8</v>
@@ -1241,7 +1265,7 @@
         <v>8</v>
       </c>
       <c r="K23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1276,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="K24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1311,7 +1335,7 @@
         <v>8</v>
       </c>
       <c r="K25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1381,7 +1405,7 @@
         <v>8</v>
       </c>
       <c r="K27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1404,7 +1428,7 @@
         <v>3829</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
         <v>7</v>
@@ -1416,7 +1440,7 @@
         <v>7</v>
       </c>
       <c r="K28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1486,7 +1510,7 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1521,7 +1545,7 @@
         <v>8</v>
       </c>
       <c r="K31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1556,7 +1580,7 @@
         <v>8</v>
       </c>
       <c r="K32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1626,7 +1650,7 @@
         <v>7</v>
       </c>
       <c r="K34" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1661,7 +1685,7 @@
         <v>8</v>
       </c>
       <c r="K35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1696,7 +1720,7 @@
         <v>8</v>
       </c>
       <c r="K36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1719,7 +1743,7 @@
         <v>2268</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="s">
         <v>8</v>
@@ -1731,7 +1755,7 @@
         <v>8</v>
       </c>
       <c r="K37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1766,7 +1790,7 @@
         <v>8</v>
       </c>
       <c r="K38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1801,6 +1825,3716 @@
         <v>8</v>
       </c>
       <c r="K39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>680000</v>
+      </c>
+      <c r="B40">
+        <v>1475</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>1980</v>
+      </c>
+      <c r="F40">
+        <v>3253</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1305000</v>
+      </c>
+      <c r="B41">
+        <v>1756</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1986</v>
+      </c>
+      <c r="F41">
+        <v>6700</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>468000</v>
+      </c>
+      <c r="B42">
+        <v>900</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1963</v>
+      </c>
+      <c r="F42">
+        <v>914</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" t="s">
+        <v>8</v>
+      </c>
+      <c r="K42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>205000</v>
+      </c>
+      <c r="B43">
+        <v>940</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>2017</v>
+      </c>
+      <c r="F43">
+        <v>940</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" t="s">
+        <v>8</v>
+      </c>
+      <c r="K43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>699900</v>
+      </c>
+      <c r="B44">
+        <v>1296</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>2021</v>
+      </c>
+      <c r="F44">
+        <v>1296</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>650000</v>
+      </c>
+      <c r="B45">
+        <v>1148</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1953</v>
+      </c>
+      <c r="F45">
+        <v>8102</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" t="s">
+        <v>8</v>
+      </c>
+      <c r="K45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1100000</v>
+      </c>
+      <c r="B46">
+        <v>1235</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>1890</v>
+      </c>
+      <c r="F46">
+        <v>5227</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" t="s">
+        <v>8</v>
+      </c>
+      <c r="K46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1765000</v>
+      </c>
+      <c r="B47">
+        <v>2422</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>1950</v>
+      </c>
+      <c r="F47">
+        <v>10366</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" t="s">
+        <v>8</v>
+      </c>
+      <c r="K47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>565000</v>
+      </c>
+      <c r="B48">
+        <v>1025</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>1985</v>
+      </c>
+      <c r="F48">
+        <v>1025</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1600000</v>
+      </c>
+      <c r="B49">
+        <v>2403</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>1976</v>
+      </c>
+      <c r="F49">
+        <v>9310</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
+      <c r="K49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1325000</v>
+      </c>
+      <c r="B50">
+        <v>2238</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>1993</v>
+      </c>
+      <c r="F50">
+        <v>6283</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" t="s">
+        <v>8</v>
+      </c>
+      <c r="K50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1100000</v>
+      </c>
+      <c r="B51">
+        <v>1235</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>1890</v>
+      </c>
+      <c r="F51">
+        <v>5200</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" t="s">
+        <v>8</v>
+      </c>
+      <c r="K51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1300000</v>
+      </c>
+      <c r="B52">
+        <v>2079</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>1950</v>
+      </c>
+      <c r="F52">
+        <v>14810</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" t="s">
+        <v>8</v>
+      </c>
+      <c r="K52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>455000</v>
+      </c>
+      <c r="B53">
+        <v>900</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1963</v>
+      </c>
+      <c r="F53">
+        <v>900</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" t="s">
+        <v>8</v>
+      </c>
+      <c r="K53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1500000</v>
+      </c>
+      <c r="B54">
+        <v>2530</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>1959</v>
+      </c>
+      <c r="F54">
+        <v>6750</v>
+      </c>
+      <c r="G54">
+        <v>6</v>
+      </c>
+      <c r="H54" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" t="s">
+        <v>8</v>
+      </c>
+      <c r="K54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1150000</v>
+      </c>
+      <c r="B55">
+        <v>1630</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>1994</v>
+      </c>
+      <c r="F55">
+        <v>6102</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" t="s">
+        <v>8</v>
+      </c>
+      <c r="K55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1001184</v>
+      </c>
+      <c r="B56">
+        <v>1722</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>2021</v>
+      </c>
+      <c r="F56">
+        <v>5000</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" t="s">
+        <v>8</v>
+      </c>
+      <c r="K56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>305000</v>
+      </c>
+      <c r="B57">
+        <v>1248</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>1974</v>
+      </c>
+      <c r="F57">
+        <v>3484</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" t="s">
+        <v>7</v>
+      </c>
+      <c r="J57" t="s">
+        <v>7</v>
+      </c>
+      <c r="K57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>941000</v>
+      </c>
+      <c r="B58">
+        <v>1888</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1949</v>
+      </c>
+      <c r="F58">
+        <v>6789</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" t="s">
+        <v>8</v>
+      </c>
+      <c r="K58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1300000</v>
+      </c>
+      <c r="B59">
+        <v>1858</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59">
+        <v>1959</v>
+      </c>
+      <c r="F59">
+        <v>9000</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" t="s">
+        <v>8</v>
+      </c>
+      <c r="J59" t="s">
+        <v>8</v>
+      </c>
+      <c r="K59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>185000</v>
+      </c>
+      <c r="B60">
+        <v>760</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1967</v>
+      </c>
+      <c r="F60">
+        <v>2614</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>755900</v>
+      </c>
+      <c r="B61">
+        <v>1726</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>2021</v>
+      </c>
+      <c r="F61">
+        <v>4500</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" t="s">
+        <v>8</v>
+      </c>
+      <c r="K61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>305000</v>
+      </c>
+      <c r="B62">
+        <v>1344</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>1974</v>
+      </c>
+      <c r="F62">
+        <v>3325</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" t="s">
+        <v>7</v>
+      </c>
+      <c r="J62" t="s">
+        <v>7</v>
+      </c>
+      <c r="K62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1800000</v>
+      </c>
+      <c r="B63">
+        <v>3233</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>1989</v>
+      </c>
+      <c r="F63">
+        <v>8276</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>7</v>
+      </c>
+      <c r="I63" t="s">
+        <v>7</v>
+      </c>
+      <c r="J63" t="s">
+        <v>7</v>
+      </c>
+      <c r="K63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>139000</v>
+      </c>
+      <c r="B64">
+        <v>572</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>2019</v>
+      </c>
+      <c r="F64">
+        <v>572</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" t="s">
+        <v>8</v>
+      </c>
+      <c r="K64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1100125</v>
+      </c>
+      <c r="B65">
+        <v>2234</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>2003</v>
+      </c>
+      <c r="F65">
+        <v>4545</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" t="s">
+        <v>8</v>
+      </c>
+      <c r="K65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>875000</v>
+      </c>
+      <c r="B66">
+        <v>1482</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>1978</v>
+      </c>
+      <c r="F66">
+        <v>4988</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66" t="s">
+        <v>8</v>
+      </c>
+      <c r="I66" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" t="s">
+        <v>8</v>
+      </c>
+      <c r="K66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>645000</v>
+      </c>
+      <c r="B67">
+        <v>1311</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>1996</v>
+      </c>
+      <c r="F67">
+        <v>1306</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" t="s">
+        <v>7</v>
+      </c>
+      <c r="K67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>416000</v>
+      </c>
+      <c r="B68">
+        <v>751</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1987</v>
+      </c>
+      <c r="F68">
+        <v>751</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" t="s">
+        <v>7</v>
+      </c>
+      <c r="K68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>603000</v>
+      </c>
+      <c r="B69">
+        <v>1369</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>2.5</v>
+      </c>
+      <c r="E69">
+        <v>1982</v>
+      </c>
+      <c r="F69">
+        <v>1369</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>8</v>
+      </c>
+      <c r="I69" t="s">
+        <v>7</v>
+      </c>
+      <c r="J69" t="s">
+        <v>8</v>
+      </c>
+      <c r="K69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>915000</v>
+      </c>
+      <c r="B70">
+        <v>1700</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>1954</v>
+      </c>
+      <c r="F70">
+        <v>7421</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>8</v>
+      </c>
+      <c r="I70" t="s">
+        <v>7</v>
+      </c>
+      <c r="J70" t="s">
+        <v>8</v>
+      </c>
+      <c r="K70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>790000</v>
+      </c>
+      <c r="B71">
+        <v>1638</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>1996</v>
+      </c>
+      <c r="F71">
+        <v>4655</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" t="s">
+        <v>8</v>
+      </c>
+      <c r="K71" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>115000</v>
+      </c>
+      <c r="B72">
+        <v>749</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>1971</v>
+      </c>
+      <c r="F72">
+        <v>749</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" t="s">
+        <v>7</v>
+      </c>
+      <c r="J72" t="s">
+        <v>8</v>
+      </c>
+      <c r="K72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>890000</v>
+      </c>
+      <c r="B73">
+        <v>600</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1963</v>
+      </c>
+      <c r="F73">
+        <v>4604</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" t="s">
+        <v>8</v>
+      </c>
+      <c r="J73" t="s">
+        <v>8</v>
+      </c>
+      <c r="K73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>855000</v>
+      </c>
+      <c r="B74">
+        <v>1115</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1953</v>
+      </c>
+      <c r="F74">
+        <v>6063</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+      <c r="H74" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" t="s">
+        <v>8</v>
+      </c>
+      <c r="J74" t="s">
+        <v>8</v>
+      </c>
+      <c r="K74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>530000</v>
+      </c>
+      <c r="B75">
+        <v>1452</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>1966</v>
+      </c>
+      <c r="F75">
+        <v>1188</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75" t="s">
+        <v>7</v>
+      </c>
+      <c r="I75" t="s">
+        <v>7</v>
+      </c>
+      <c r="J75" t="s">
+        <v>7</v>
+      </c>
+      <c r="K75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1100000</v>
+      </c>
+      <c r="B76">
+        <v>1214</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>1960</v>
+      </c>
+      <c r="F76">
+        <v>5904</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76" t="s">
+        <v>8</v>
+      </c>
+      <c r="I76" t="s">
+        <v>8</v>
+      </c>
+      <c r="J76" t="s">
+        <v>8</v>
+      </c>
+      <c r="K76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>800000</v>
+      </c>
+      <c r="B77">
+        <v>1247</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>1986</v>
+      </c>
+      <c r="F77">
+        <v>1247</v>
+      </c>
+      <c r="G77">
+        <v>2</v>
+      </c>
+      <c r="H77" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" t="s">
+        <v>7</v>
+      </c>
+      <c r="J77" t="s">
+        <v>8</v>
+      </c>
+      <c r="K77" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>640000</v>
+      </c>
+      <c r="B78">
+        <v>1396</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>2.5</v>
+      </c>
+      <c r="E78">
+        <v>1994</v>
+      </c>
+      <c r="F78">
+        <v>1393</v>
+      </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
+      <c r="H78" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" t="s">
+        <v>7</v>
+      </c>
+      <c r="J78" t="s">
+        <v>8</v>
+      </c>
+      <c r="K78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>652500</v>
+      </c>
+      <c r="B79">
+        <v>1365</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>1982</v>
+      </c>
+      <c r="F79">
+        <v>1365</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+      <c r="H79" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79" t="s">
+        <v>7</v>
+      </c>
+      <c r="J79" t="s">
+        <v>8</v>
+      </c>
+      <c r="K79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>280000</v>
+      </c>
+      <c r="B80">
+        <v>1069</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>2004</v>
+      </c>
+      <c r="F80">
+        <v>1069</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>7</v>
+      </c>
+      <c r="I80" t="s">
+        <v>7</v>
+      </c>
+      <c r="J80" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>880000</v>
+      </c>
+      <c r="B81">
+        <v>1160</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1949</v>
+      </c>
+      <c r="F81">
+        <v>5000</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" t="s">
+        <v>7</v>
+      </c>
+      <c r="J81" t="s">
+        <v>8</v>
+      </c>
+      <c r="K81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>882000</v>
+      </c>
+      <c r="B82">
+        <v>1800</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>1966</v>
+      </c>
+      <c r="F82">
+        <v>6900</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="H82" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" t="s">
+        <v>7</v>
+      </c>
+      <c r="J82" t="s">
+        <v>8</v>
+      </c>
+      <c r="K82" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1245000</v>
+      </c>
+      <c r="B83">
+        <v>1604</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83">
+        <v>1961</v>
+      </c>
+      <c r="F83">
+        <v>13504</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83" t="s">
+        <v>7</v>
+      </c>
+      <c r="I83" t="s">
+        <v>7</v>
+      </c>
+      <c r="J83" t="s">
+        <v>8</v>
+      </c>
+      <c r="K83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>350000</v>
+      </c>
+      <c r="B84">
+        <v>1160</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>2004</v>
+      </c>
+      <c r="F84">
+        <v>1160</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" t="s">
+        <v>8</v>
+      </c>
+      <c r="I84" t="s">
+        <v>7</v>
+      </c>
+      <c r="J84" t="s">
+        <v>7</v>
+      </c>
+      <c r="K84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>560000</v>
+      </c>
+      <c r="B85">
+        <v>940</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>1985</v>
+      </c>
+      <c r="F85">
+        <v>940</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85" t="s">
+        <v>8</v>
+      </c>
+      <c r="I85" t="s">
+        <v>8</v>
+      </c>
+      <c r="J85" t="s">
+        <v>7</v>
+      </c>
+      <c r="K85" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>990000</v>
+      </c>
+      <c r="B86">
+        <v>1593</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>2.5</v>
+      </c>
+      <c r="E86">
+        <v>1950</v>
+      </c>
+      <c r="F86">
+        <v>14810</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" t="s">
+        <v>8</v>
+      </c>
+      <c r="J86" t="s">
+        <v>8</v>
+      </c>
+      <c r="K86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>527500</v>
+      </c>
+      <c r="B87">
+        <v>1138</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>1966</v>
+      </c>
+      <c r="F87">
+        <v>1126</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
+        <v>8</v>
+      </c>
+      <c r="I87" t="s">
+        <v>7</v>
+      </c>
+      <c r="J87" t="s">
+        <v>7</v>
+      </c>
+      <c r="K87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1523000</v>
+      </c>
+      <c r="B88">
+        <v>2547</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88">
+        <v>2013</v>
+      </c>
+      <c r="F88">
+        <v>8818</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="H88" t="s">
+        <v>8</v>
+      </c>
+      <c r="I88" t="s">
+        <v>7</v>
+      </c>
+      <c r="J88" t="s">
+        <v>8</v>
+      </c>
+      <c r="K88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1100000</v>
+      </c>
+      <c r="B89">
+        <v>1216</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>1949</v>
+      </c>
+      <c r="F89">
+        <v>7500</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89" t="s">
+        <v>8</v>
+      </c>
+      <c r="I89" t="s">
+        <v>7</v>
+      </c>
+      <c r="J89" t="s">
+        <v>8</v>
+      </c>
+      <c r="K89" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>240000</v>
+      </c>
+      <c r="B90">
+        <v>1144</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>1928</v>
+      </c>
+      <c r="F90">
+        <v>6300</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90" t="s">
+        <v>8</v>
+      </c>
+      <c r="I90" t="s">
+        <v>8</v>
+      </c>
+      <c r="J90" t="s">
+        <v>8</v>
+      </c>
+      <c r="K90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>650000</v>
+      </c>
+      <c r="B91">
+        <v>918</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>1975</v>
+      </c>
+      <c r="F91">
+        <v>918</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91" t="s">
+        <v>7</v>
+      </c>
+      <c r="I91" t="s">
+        <v>7</v>
+      </c>
+      <c r="J91" t="s">
+        <v>7</v>
+      </c>
+      <c r="K91" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1040000</v>
+      </c>
+      <c r="B92">
+        <v>1785</v>
+      </c>
+      <c r="C92">
+        <v>4</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+      <c r="E92">
+        <v>1969</v>
+      </c>
+      <c r="F92">
+        <v>2750</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" t="s">
+        <v>8</v>
+      </c>
+      <c r="J92" t="s">
+        <v>8</v>
+      </c>
+      <c r="K92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1300000</v>
+      </c>
+      <c r="B93">
+        <v>2122</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93">
+        <v>2019</v>
+      </c>
+      <c r="F93">
+        <v>5000</v>
+      </c>
+      <c r="G93">
+        <v>3</v>
+      </c>
+      <c r="H93" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" t="s">
+        <v>7</v>
+      </c>
+      <c r="J93" t="s">
+        <v>8</v>
+      </c>
+      <c r="K93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>880000</v>
+      </c>
+      <c r="B94">
+        <v>975</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1922</v>
+      </c>
+      <c r="F94">
+        <v>7250</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94" t="s">
+        <v>8</v>
+      </c>
+      <c r="I94" t="s">
+        <v>8</v>
+      </c>
+      <c r="J94" t="s">
+        <v>8</v>
+      </c>
+      <c r="K94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1660000</v>
+      </c>
+      <c r="B95">
+        <v>4292</v>
+      </c>
+      <c r="C95">
+        <v>5</v>
+      </c>
+      <c r="D95">
+        <v>4</v>
+      </c>
+      <c r="E95">
+        <v>1961</v>
+      </c>
+      <c r="F95">
+        <v>13939</v>
+      </c>
+      <c r="G95">
+        <v>5</v>
+      </c>
+      <c r="H95" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" t="s">
+        <v>7</v>
+      </c>
+      <c r="J95" t="s">
+        <v>8</v>
+      </c>
+      <c r="K95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>699000</v>
+      </c>
+      <c r="B96">
+        <v>1410</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96">
+        <v>2009</v>
+      </c>
+      <c r="F96">
+        <v>1410</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+      <c r="H96" t="s">
+        <v>7</v>
+      </c>
+      <c r="I96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J96" t="s">
+        <v>8</v>
+      </c>
+      <c r="K96" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1355555</v>
+      </c>
+      <c r="B97">
+        <v>2217</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97">
+        <v>1991</v>
+      </c>
+      <c r="F97">
+        <v>4500</v>
+      </c>
+      <c r="G97">
+        <v>4</v>
+      </c>
+      <c r="H97" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" t="s">
+        <v>7</v>
+      </c>
+      <c r="J97" t="s">
+        <v>8</v>
+      </c>
+      <c r="K97" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>2000000</v>
+      </c>
+      <c r="B98">
+        <v>3500</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>2.75</v>
+      </c>
+      <c r="E98">
+        <v>1999</v>
+      </c>
+      <c r="F98">
+        <v>9957</v>
+      </c>
+      <c r="G98">
+        <v>3</v>
+      </c>
+      <c r="H98" t="s">
+        <v>8</v>
+      </c>
+      <c r="I98" t="s">
+        <v>7</v>
+      </c>
+      <c r="J98" t="s">
+        <v>8</v>
+      </c>
+      <c r="K98" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>565000</v>
+      </c>
+      <c r="B99">
+        <v>1050</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99">
+        <v>1985</v>
+      </c>
+      <c r="F99">
+        <v>1034</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99" t="s">
+        <v>8</v>
+      </c>
+      <c r="I99" t="s">
+        <v>8</v>
+      </c>
+      <c r="J99" t="s">
+        <v>7</v>
+      </c>
+      <c r="K99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1100000</v>
+      </c>
+      <c r="B100">
+        <v>2087</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>1986</v>
+      </c>
+      <c r="F100">
+        <v>8058</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+      <c r="H100" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" t="s">
+        <v>8</v>
+      </c>
+      <c r="J100" t="s">
+        <v>8</v>
+      </c>
+      <c r="K100" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>145000</v>
+      </c>
+      <c r="B101">
+        <v>800</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <v>2</v>
+      </c>
+      <c r="E101">
+        <v>1974</v>
+      </c>
+      <c r="F101">
+        <v>800</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>8</v>
+      </c>
+      <c r="I101" t="s">
+        <v>7</v>
+      </c>
+      <c r="J101" t="s">
+        <v>7</v>
+      </c>
+      <c r="K101" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>395000</v>
+      </c>
+      <c r="B102">
+        <v>736</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>2007</v>
+      </c>
+      <c r="F102">
+        <v>736</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>8</v>
+      </c>
+      <c r="I102" t="s">
+        <v>7</v>
+      </c>
+      <c r="J102" t="s">
+        <v>8</v>
+      </c>
+      <c r="K102" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>620000</v>
+      </c>
+      <c r="B103">
+        <v>972</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>1910</v>
+      </c>
+      <c r="F103">
+        <v>2789</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103" t="s">
+        <v>8</v>
+      </c>
+      <c r="I103" t="s">
+        <v>8</v>
+      </c>
+      <c r="J103" t="s">
+        <v>8</v>
+      </c>
+      <c r="K103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>660000</v>
+      </c>
+      <c r="B104">
+        <v>1658</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>3</v>
+      </c>
+      <c r="E104">
+        <v>2010</v>
+      </c>
+      <c r="F104">
+        <v>1659</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+      <c r="H104" t="s">
+        <v>7</v>
+      </c>
+      <c r="I104" t="s">
+        <v>7</v>
+      </c>
+      <c r="J104" t="s">
+        <v>8</v>
+      </c>
+      <c r="K104" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>880000</v>
+      </c>
+      <c r="B105">
+        <v>1799</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105">
+        <v>1977</v>
+      </c>
+      <c r="F105">
+        <v>5000</v>
+      </c>
+      <c r="G105">
+        <v>2</v>
+      </c>
+      <c r="H105" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" t="s">
+        <v>7</v>
+      </c>
+      <c r="J105" t="s">
+        <v>8</v>
+      </c>
+      <c r="K105" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>900000</v>
+      </c>
+      <c r="B106">
+        <v>2026</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>3</v>
+      </c>
+      <c r="E106">
+        <v>2004</v>
+      </c>
+      <c r="F106">
+        <v>6416</v>
+      </c>
+      <c r="G106">
+        <v>4</v>
+      </c>
+      <c r="H106" t="s">
+        <v>8</v>
+      </c>
+      <c r="I106" t="s">
+        <v>7</v>
+      </c>
+      <c r="J106" t="s">
+        <v>8</v>
+      </c>
+      <c r="K106" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>354000</v>
+      </c>
+      <c r="B107">
+        <v>1242</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107">
+        <v>2004</v>
+      </c>
+      <c r="F107">
+        <v>2600</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107" t="s">
+        <v>8</v>
+      </c>
+      <c r="I107" t="s">
+        <v>7</v>
+      </c>
+      <c r="J107" t="s">
+        <v>7</v>
+      </c>
+      <c r="K107" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>260000</v>
+      </c>
+      <c r="B108">
+        <v>1368</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>2</v>
+      </c>
+      <c r="E108">
+        <v>1971</v>
+      </c>
+      <c r="F108">
+        <v>1368</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="H108" t="s">
+        <v>8</v>
+      </c>
+      <c r="I108" t="s">
+        <v>8</v>
+      </c>
+      <c r="J108" t="s">
+        <v>7</v>
+      </c>
+      <c r="K108" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1300000</v>
+      </c>
+      <c r="B109">
+        <v>1000</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+      <c r="E109">
+        <v>1900</v>
+      </c>
+      <c r="F109">
+        <v>3301</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="H109" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" t="s">
+        <v>7</v>
+      </c>
+      <c r="J109" t="s">
+        <v>8</v>
+      </c>
+      <c r="K109" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>2200000</v>
+      </c>
+      <c r="B110">
+        <v>3214</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+      <c r="D110">
+        <v>3</v>
+      </c>
+      <c r="E110">
+        <v>1990</v>
+      </c>
+      <c r="F110">
+        <v>11326</v>
+      </c>
+      <c r="G110">
+        <v>3</v>
+      </c>
+      <c r="H110" t="s">
+        <v>8</v>
+      </c>
+      <c r="I110" t="s">
+        <v>7</v>
+      </c>
+      <c r="J110" t="s">
+        <v>8</v>
+      </c>
+      <c r="K110" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>635000</v>
+      </c>
+      <c r="B111">
+        <v>1452</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111">
+        <v>1948</v>
+      </c>
+      <c r="F111">
+        <v>5998</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="H111" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" t="s">
+        <v>7</v>
+      </c>
+      <c r="J111" t="s">
+        <v>8</v>
+      </c>
+      <c r="K111" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>690000</v>
+      </c>
+      <c r="B112">
+        <v>1389</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112">
+        <v>3</v>
+      </c>
+      <c r="E112">
+        <v>1987</v>
+      </c>
+      <c r="F112">
+        <v>1999</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+      <c r="H112" t="s">
+        <v>8</v>
+      </c>
+      <c r="I112" t="s">
+        <v>7</v>
+      </c>
+      <c r="J112" t="s">
+        <v>7</v>
+      </c>
+      <c r="K112" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>492000</v>
+      </c>
+      <c r="B113">
+        <v>850</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>1973</v>
+      </c>
+      <c r="F113">
+        <v>849.42</v>
+      </c>
+      <c r="G113">
+        <v>2</v>
+      </c>
+      <c r="H113" t="s">
+        <v>8</v>
+      </c>
+      <c r="I113" t="s">
+        <v>7</v>
+      </c>
+      <c r="J113" t="s">
+        <v>7</v>
+      </c>
+      <c r="K113" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>700000</v>
+      </c>
+      <c r="B114">
+        <v>1742</v>
+      </c>
+      <c r="C114">
+        <v>4</v>
+      </c>
+      <c r="D114">
+        <v>2</v>
+      </c>
+      <c r="E114">
+        <v>1976</v>
+      </c>
+      <c r="F114">
+        <v>4051</v>
+      </c>
+      <c r="G114">
+        <v>4</v>
+      </c>
+      <c r="H114" t="s">
+        <v>8</v>
+      </c>
+      <c r="I114" t="s">
+        <v>7</v>
+      </c>
+      <c r="J114" t="s">
+        <v>7</v>
+      </c>
+      <c r="K114" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>325000</v>
+      </c>
+      <c r="B115">
+        <v>1088</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115">
+        <v>1970</v>
+      </c>
+      <c r="F115">
+        <v>435</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115" t="s">
+        <v>8</v>
+      </c>
+      <c r="I115" t="s">
+        <v>7</v>
+      </c>
+      <c r="J115" t="s">
+        <v>8</v>
+      </c>
+      <c r="K115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1060248</v>
+      </c>
+      <c r="B116">
+        <v>2759</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
+      </c>
+      <c r="D116">
+        <v>4</v>
+      </c>
+      <c r="E116">
+        <v>2021</v>
+      </c>
+      <c r="F116">
+        <v>4878</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+      <c r="H116" t="s">
+        <v>8</v>
+      </c>
+      <c r="I116" t="s">
+        <v>7</v>
+      </c>
+      <c r="J116" t="s">
+        <v>8</v>
+      </c>
+      <c r="K116" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>886904</v>
+      </c>
+      <c r="B117">
+        <v>1904</v>
+      </c>
+      <c r="C117">
+        <v>3</v>
+      </c>
+      <c r="D117">
+        <v>3</v>
+      </c>
+      <c r="E117">
+        <v>2021</v>
+      </c>
+      <c r="F117">
+        <v>4500</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+      <c r="H117" t="s">
+        <v>7</v>
+      </c>
+      <c r="I117" t="s">
+        <v>7</v>
+      </c>
+      <c r="J117" t="s">
+        <v>8</v>
+      </c>
+      <c r="K117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>835000</v>
+      </c>
+      <c r="B118">
+        <v>2099</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118">
+        <v>3</v>
+      </c>
+      <c r="E118">
+        <v>1990</v>
+      </c>
+      <c r="F118">
+        <v>5201</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+      <c r="H118" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" t="s">
+        <v>7</v>
+      </c>
+      <c r="J118" t="s">
+        <v>8</v>
+      </c>
+      <c r="K118" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1450000</v>
+      </c>
+      <c r="B119">
+        <v>1641</v>
+      </c>
+      <c r="C119">
+        <v>4</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+      <c r="E119">
+        <v>1962</v>
+      </c>
+      <c r="F119">
+        <v>9600</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+      <c r="H119" t="s">
+        <v>8</v>
+      </c>
+      <c r="I119" t="s">
+        <v>7</v>
+      </c>
+      <c r="J119" t="s">
+        <v>8</v>
+      </c>
+      <c r="K119" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>554000</v>
+      </c>
+      <c r="B120">
+        <v>1100</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="E120">
+        <v>1980</v>
+      </c>
+      <c r="F120">
+        <v>1102</v>
+      </c>
+      <c r="G120">
+        <v>3</v>
+      </c>
+      <c r="H120" t="s">
+        <v>8</v>
+      </c>
+      <c r="I120" t="s">
+        <v>7</v>
+      </c>
+      <c r="J120" t="s">
+        <v>8</v>
+      </c>
+      <c r="K120" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>389000</v>
+      </c>
+      <c r="B121">
+        <v>1050</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121">
+        <v>2016</v>
+      </c>
+      <c r="F121">
+        <v>2600</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="H121" t="s">
+        <v>8</v>
+      </c>
+      <c r="I121" t="s">
+        <v>7</v>
+      </c>
+      <c r="J121" t="s">
+        <v>7</v>
+      </c>
+      <c r="K121" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>230000</v>
+      </c>
+      <c r="B122">
+        <v>1040</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+      <c r="E122">
+        <v>1977</v>
+      </c>
+      <c r="F122">
+        <v>2600</v>
+      </c>
+      <c r="G122">
+        <v>1</v>
+      </c>
+      <c r="H122" t="s">
+        <v>7</v>
+      </c>
+      <c r="I122" t="s">
+        <v>7</v>
+      </c>
+      <c r="J122" t="s">
+        <v>7</v>
+      </c>
+      <c r="K122" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>300000</v>
+      </c>
+      <c r="B123">
+        <v>1450</v>
+      </c>
+      <c r="C123">
+        <v>3</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <v>2015</v>
+      </c>
+      <c r="F123">
+        <v>1450</v>
+      </c>
+      <c r="G123">
+        <v>1</v>
+      </c>
+      <c r="H123" t="s">
+        <v>8</v>
+      </c>
+      <c r="I123" t="s">
+        <v>7</v>
+      </c>
+      <c r="J123" t="s">
+        <v>7</v>
+      </c>
+      <c r="K123" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1225000</v>
+      </c>
+      <c r="B124">
+        <v>2100</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>1985</v>
+      </c>
+      <c r="F124">
+        <v>6699</v>
+      </c>
+      <c r="G124">
+        <v>2</v>
+      </c>
+      <c r="H124" t="s">
+        <v>8</v>
+      </c>
+      <c r="I124" t="s">
+        <v>7</v>
+      </c>
+      <c r="J124" t="s">
+        <v>8</v>
+      </c>
+      <c r="K124" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>950000</v>
+      </c>
+      <c r="B125">
+        <v>770</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>1959</v>
+      </c>
+      <c r="F125">
+        <v>4901</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125" t="s">
+        <v>8</v>
+      </c>
+      <c r="I125" t="s">
+        <v>7</v>
+      </c>
+      <c r="J125" t="s">
+        <v>8</v>
+      </c>
+      <c r="K125" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1135000</v>
+      </c>
+      <c r="B126">
+        <v>1226</v>
+      </c>
+      <c r="C126">
+        <v>3</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>1935</v>
+      </c>
+      <c r="F126">
+        <v>5000</v>
+      </c>
+      <c r="G126">
+        <v>2</v>
+      </c>
+      <c r="H126" t="s">
+        <v>8</v>
+      </c>
+      <c r="I126" t="s">
+        <v>8</v>
+      </c>
+      <c r="J126" t="s">
+        <v>8</v>
+      </c>
+      <c r="K126" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>970000</v>
+      </c>
+      <c r="B127">
+        <v>1224</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>1920</v>
+      </c>
+      <c r="F127">
+        <v>3824</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+      <c r="H127" t="s">
+        <v>8</v>
+      </c>
+      <c r="I127" t="s">
+        <v>7</v>
+      </c>
+      <c r="J127" t="s">
+        <v>8</v>
+      </c>
+      <c r="K127" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1846155</v>
+      </c>
+      <c r="B128">
+        <v>2044</v>
+      </c>
+      <c r="C128">
+        <v>6</v>
+      </c>
+      <c r="D128">
+        <v>4</v>
+      </c>
+      <c r="E128">
+        <v>1950</v>
+      </c>
+      <c r="F128">
+        <v>5000</v>
+      </c>
+      <c r="G128">
+        <v>1</v>
+      </c>
+      <c r="H128" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" t="s">
+        <v>7</v>
+      </c>
+      <c r="J128" t="s">
+        <v>8</v>
+      </c>
+      <c r="K128" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1525000</v>
+      </c>
+      <c r="B129">
+        <v>2807</v>
+      </c>
+      <c r="C129">
+        <v>5</v>
+      </c>
+      <c r="D129">
+        <v>3</v>
+      </c>
+      <c r="E129">
+        <v>2002</v>
+      </c>
+      <c r="F129">
+        <v>6751</v>
+      </c>
+      <c r="G129">
+        <v>2</v>
+      </c>
+      <c r="H129" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" t="s">
+        <v>7</v>
+      </c>
+      <c r="J129" t="s">
+        <v>8</v>
+      </c>
+      <c r="K129" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>399000</v>
+      </c>
+      <c r="B130">
+        <v>1840</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>1975</v>
+      </c>
+      <c r="F130">
+        <v>3001</v>
+      </c>
+      <c r="G130">
+        <v>3</v>
+      </c>
+      <c r="H130" t="s">
+        <v>7</v>
+      </c>
+      <c r="I130" t="s">
+        <v>7</v>
+      </c>
+      <c r="J130" t="s">
+        <v>7</v>
+      </c>
+      <c r="K130" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1825000</v>
+      </c>
+      <c r="B131">
+        <v>3022</v>
+      </c>
+      <c r="C131">
+        <v>3</v>
+      </c>
+      <c r="D131">
+        <v>3</v>
+      </c>
+      <c r="E131">
+        <v>1990</v>
+      </c>
+      <c r="F131">
+        <v>9226</v>
+      </c>
+      <c r="G131">
+        <v>2</v>
+      </c>
+      <c r="H131" t="s">
+        <v>8</v>
+      </c>
+      <c r="I131" t="s">
+        <v>8</v>
+      </c>
+      <c r="J131" t="s">
+        <v>8</v>
+      </c>
+      <c r="K131" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1635000</v>
+      </c>
+      <c r="B132">
+        <v>2529</v>
+      </c>
+      <c r="C132">
+        <v>5</v>
+      </c>
+      <c r="D132">
+        <v>4</v>
+      </c>
+      <c r="E132">
+        <v>1966</v>
+      </c>
+      <c r="F132">
+        <v>8241</v>
+      </c>
+      <c r="G132">
+        <v>2</v>
+      </c>
+      <c r="H132" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" t="s">
+        <v>7</v>
+      </c>
+      <c r="J132" t="s">
+        <v>8</v>
+      </c>
+      <c r="K132" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>493000</v>
+      </c>
+      <c r="B133">
+        <v>1001</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133">
+        <v>2</v>
+      </c>
+      <c r="E133">
+        <v>1973</v>
+      </c>
+      <c r="F133">
+        <v>1001</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+      <c r="H133" t="s">
+        <v>8</v>
+      </c>
+      <c r="I133" t="s">
+        <v>7</v>
+      </c>
+      <c r="J133" t="s">
+        <v>7</v>
+      </c>
+      <c r="K133" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1265000</v>
+      </c>
+      <c r="B134">
+        <v>1542</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+      <c r="D134">
+        <v>3</v>
+      </c>
+      <c r="E134">
+        <v>1962</v>
+      </c>
+      <c r="F134">
+        <v>84071</v>
+      </c>
+      <c r="G134">
+        <v>2</v>
+      </c>
+      <c r="H134" t="s">
+        <v>8</v>
+      </c>
+      <c r="I134" t="s">
+        <v>7</v>
+      </c>
+      <c r="J134" t="s">
+        <v>8</v>
+      </c>
+      <c r="K134" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>300000</v>
+      </c>
+      <c r="B135">
+        <v>1638</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>3</v>
+      </c>
+      <c r="E135">
+        <v>2022</v>
+      </c>
+      <c r="F135">
+        <v>1000</v>
+      </c>
+      <c r="G135">
+        <v>2</v>
+      </c>
+      <c r="H135" t="s">
+        <v>7</v>
+      </c>
+      <c r="I135" t="s">
+        <v>7</v>
+      </c>
+      <c r="J135" t="s">
+        <v>8</v>
+      </c>
+      <c r="K135" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>615000</v>
+      </c>
+      <c r="B136">
+        <v>1243</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+      <c r="E136">
+        <v>1980</v>
+      </c>
+      <c r="F136">
+        <v>3432</v>
+      </c>
+      <c r="G136">
+        <v>3</v>
+      </c>
+      <c r="H136" t="s">
+        <v>8</v>
+      </c>
+      <c r="I136" t="s">
+        <v>7</v>
+      </c>
+      <c r="J136" t="s">
+        <v>8</v>
+      </c>
+      <c r="K136" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>485000</v>
+      </c>
+      <c r="B137">
+        <v>971</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137">
+        <v>2</v>
+      </c>
+      <c r="E137">
+        <v>1984</v>
+      </c>
+      <c r="F137">
+        <v>971.39</v>
+      </c>
+      <c r="G137">
+        <v>2</v>
+      </c>
+      <c r="H137" t="s">
+        <v>8</v>
+      </c>
+      <c r="I137" t="s">
+        <v>7</v>
+      </c>
+      <c r="J137" t="s">
+        <v>8</v>
+      </c>
+      <c r="K137" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>850000</v>
+      </c>
+      <c r="B138">
+        <v>1997</v>
+      </c>
+      <c r="C138">
+        <v>4</v>
+      </c>
+      <c r="D138">
+        <v>2</v>
+      </c>
+      <c r="E138">
+        <v>1961</v>
+      </c>
+      <c r="F138">
+        <v>12632</v>
+      </c>
+      <c r="G138">
+        <v>2</v>
+      </c>
+      <c r="H138" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138" t="s">
+        <v>7</v>
+      </c>
+      <c r="J138" t="s">
+        <v>8</v>
+      </c>
+      <c r="K138" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>1200000</v>
+      </c>
+      <c r="B139">
+        <v>1478</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>2</v>
+      </c>
+      <c r="E139">
+        <v>1989</v>
+      </c>
+      <c r="F139">
+        <v>6163</v>
+      </c>
+      <c r="G139">
+        <v>2</v>
+      </c>
+      <c r="H139" t="s">
+        <v>8</v>
+      </c>
+      <c r="I139" t="s">
+        <v>8</v>
+      </c>
+      <c r="J139" t="s">
+        <v>8</v>
+      </c>
+      <c r="K139" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>2295000</v>
+      </c>
+      <c r="B140">
+        <v>3293</v>
+      </c>
+      <c r="C140">
+        <v>3</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+      <c r="E140">
+        <v>2000</v>
+      </c>
+      <c r="F140">
+        <v>108900</v>
+      </c>
+      <c r="G140">
+        <v>3</v>
+      </c>
+      <c r="H140" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" t="s">
+        <v>7</v>
+      </c>
+      <c r="J140" t="s">
+        <v>8</v>
+      </c>
+      <c r="K140" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>220000</v>
+      </c>
+      <c r="B141">
+        <v>1040</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
+      <c r="E141">
+        <v>1993</v>
+      </c>
+      <c r="F141">
+        <v>2700</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
+      <c r="H141" t="s">
+        <v>8</v>
+      </c>
+      <c r="I141" t="s">
+        <v>8</v>
+      </c>
+      <c r="J141" t="s">
+        <v>8</v>
+      </c>
+      <c r="K141" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>306000</v>
+      </c>
+      <c r="B142">
+        <v>1440</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
+      <c r="E142">
+        <v>1971</v>
+      </c>
+      <c r="F142">
+        <v>1440</v>
+      </c>
+      <c r="G142">
+        <v>2</v>
+      </c>
+      <c r="H142" t="s">
+        <v>8</v>
+      </c>
+      <c r="I142" t="s">
+        <v>7</v>
+      </c>
+      <c r="J142" t="s">
+        <v>7</v>
+      </c>
+      <c r="K142" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>645000</v>
+      </c>
+      <c r="B143">
+        <v>1389</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143">
+        <v>1987</v>
+      </c>
+      <c r="F143">
+        <v>1999</v>
+      </c>
+      <c r="G143">
+        <v>2</v>
+      </c>
+      <c r="H143" t="s">
+        <v>8</v>
+      </c>
+      <c r="I143" t="s">
+        <v>7</v>
+      </c>
+      <c r="J143" t="s">
+        <v>7</v>
+      </c>
+      <c r="K143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>895000</v>
+      </c>
+      <c r="B144">
+        <v>1904</v>
+      </c>
+      <c r="C144">
+        <v>3</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+      <c r="E144">
+        <v>2021</v>
+      </c>
+      <c r="F144">
+        <v>3737</v>
+      </c>
+      <c r="G144">
+        <v>2</v>
+      </c>
+      <c r="H144" t="s">
+        <v>7</v>
+      </c>
+      <c r="I144" t="s">
+        <v>7</v>
+      </c>
+      <c r="J144" t="s">
+        <v>8</v>
+      </c>
+      <c r="K144" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>589000</v>
+      </c>
+      <c r="B145">
+        <v>1174</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>2</v>
+      </c>
+      <c r="E145">
+        <v>2019</v>
+      </c>
+      <c r="F145">
+        <v>1240</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+      <c r="H145" t="s">
+        <v>8</v>
+      </c>
+      <c r="I145" t="s">
+        <v>8</v>
+      </c>
+      <c r="J145" t="s">
+        <v>8</v>
+      </c>
+      <c r="K145" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>